<commit_message>
Incorporate updated transportation files from RMI
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/jshepard/desktop/beyondcarbon/data/output/eps/va/trans/bhnvfeal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0773C785-DA33-9946-BEC6-451AA7B186B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD955EF-6633-2D4E-956E-FC0EBE60C4DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" tabRatio="742" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="742" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -7041,16 +7041,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="10">
-        <v>2.8879999999999999E-3</v>
+        <v>1.362816616770287E-3</v>
       </c>
       <c r="C4" s="10">
-        <v>4.5399999999999998E-4</v>
+        <v>1.79343314551659E-3</v>
       </c>
       <c r="D4" s="11">
-        <v>6.0700000000000001E-4</v>
+        <v>1.5590676482152321E-4</v>
       </c>
       <c r="E4" s="11">
-        <v>6.3699999999999998E-4</v>
+        <v>8.0444857169030375E-4</v>
       </c>
       <c r="F4" s="11">
         <v>0</v>
@@ -7059,7 +7059,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="11">
-        <v>0</v>
+        <v>2.4133457150709108E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
@@ -7093,16 +7093,16 @@
         <v>11</v>
       </c>
       <c r="B6" s="10">
-        <v>1.7899999999999999E-3</v>
+        <v>1.397782879998018E-3</v>
       </c>
       <c r="C6" s="10">
-        <v>1.951E-3</v>
+        <v>4.8101686276135923E-4</v>
       </c>
       <c r="D6" s="10">
-        <v>1.951E-3</v>
+        <v>4.8101686276135923E-4</v>
       </c>
       <c r="E6" s="11">
-        <v>1.951E-3</v>
+        <v>4.8101686276135923E-4</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -7111,7 +7111,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="11">
-        <v>5.8529999999999997E-3</v>
+        <v>1.4430505882840775E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15">
@@ -7197,25 +7197,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="14">
-        <v>3.6491154123730247E-4</v>
+        <v>0</v>
       </c>
       <c r="C12" s="14">
-        <v>1.1460031873568179E-4</v>
+        <v>0</v>
       </c>
       <c r="D12" s="14">
-        <v>1.1460031873568179E-4</v>
+        <v>0</v>
       </c>
       <c r="E12" s="14">
-        <v>1.1460031873568179E-4</v>
+        <v>0</v>
       </c>
       <c r="F12" s="14">
-        <v>2.5227149111157316E-4</v>
+        <v>0</v>
       </c>
       <c r="G12" s="14">
-        <v>8.8815247020153392E-5</v>
+        <v>0</v>
       </c>
       <c r="H12" s="14">
-        <v>3.438009562070453E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15">
@@ -7275,16 +7275,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="14">
-        <v>5.8902990158970474E-3</v>
+        <v>5.8899633596941527E-3</v>
       </c>
       <c r="C15" s="14">
-        <v>1.833E-3</v>
+        <v>1.832895547268781E-3</v>
       </c>
       <c r="D15" s="14">
-        <v>1.833E-3</v>
+        <v>1.832895547268781E-3</v>
       </c>
       <c r="E15" s="14">
-        <v>1.833E-3</v>
+        <v>1.832895547268781E-3</v>
       </c>
       <c r="F15" s="14">
         <v>0</v>
@@ -7293,7 +7293,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="14">
-        <v>5.4989999999999995E-3</v>
+        <v>5.4986866418063425E-3</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15">
@@ -7301,16 +7301,16 @@
         <v>12</v>
       </c>
       <c r="B16" s="14">
-        <v>0.11579302198625165</v>
+        <v>1.580720948786267E-2</v>
       </c>
       <c r="C16" s="14">
-        <v>3.6033588231764058E-2</v>
+        <v>4.9190397487553798E-3</v>
       </c>
       <c r="D16" s="14">
-        <v>3.6033588231764058E-2</v>
+        <v>4.9190397487553798E-3</v>
       </c>
       <c r="E16" s="14">
-        <v>3.6033588231764058E-2</v>
+        <v>4.9190397487553798E-3</v>
       </c>
       <c r="F16" s="14">
         <v>0</v>
@@ -7319,7 +7319,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="14">
-        <v>0.10810076469529216</v>
+        <v>1.4757119246266137E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15">

</xml_diff>

<commit_message>
Additional RMI edits on transportation files
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\trans\BHNVFEAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/jshepard/desktop/beyondcarbon/data/output/eps/va/trans/bhnvfeal/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9D33E7-9D23-AB49-8BAB-81031F94ED9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" tabRatio="742"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12640" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -44,7 +45,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -151,7 +152,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1043,160 +1044,160 @@
     <xf numFmtId="0" fontId="41" fillId="3" borderId="0" xfId="153" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="154">
-    <cellStyle name="20% - Accent1 2" xfId="8"/>
-    <cellStyle name="20% - Accent2 2" xfId="9"/>
-    <cellStyle name="20% - Accent3 2" xfId="10"/>
-    <cellStyle name="20% - Accent4 2" xfId="11"/>
-    <cellStyle name="20% - Accent5 2" xfId="12"/>
-    <cellStyle name="20% - Accent6 2" xfId="13"/>
-    <cellStyle name="40% - Accent1 2" xfId="14"/>
-    <cellStyle name="40% - Accent2 2" xfId="15"/>
-    <cellStyle name="40% - Accent3 2" xfId="16"/>
-    <cellStyle name="40% - Accent4 2" xfId="17"/>
-    <cellStyle name="40% - Accent5 2" xfId="18"/>
-    <cellStyle name="40% - Accent6 2" xfId="19"/>
-    <cellStyle name="60% - Accent1 2" xfId="20"/>
-    <cellStyle name="60% - Accent2 2" xfId="21"/>
-    <cellStyle name="60% - Accent3 2" xfId="22"/>
-    <cellStyle name="60% - Accent4 2" xfId="23"/>
-    <cellStyle name="60% - Accent5 2" xfId="24"/>
-    <cellStyle name="60% - Accent6 2" xfId="25"/>
-    <cellStyle name="Accent1 2" xfId="26"/>
-    <cellStyle name="Accent2 2" xfId="27"/>
-    <cellStyle name="Accent3 2" xfId="28"/>
-    <cellStyle name="Accent4 2" xfId="29"/>
-    <cellStyle name="Accent5 2" xfId="30"/>
-    <cellStyle name="Accent6 2" xfId="31"/>
-    <cellStyle name="Bad 2" xfId="32"/>
-    <cellStyle name="Body: normal cell" xfId="4"/>
-    <cellStyle name="Body: normal cell 2" xfId="33"/>
-    <cellStyle name="Calculation 2" xfId="34"/>
-    <cellStyle name="Check Cell 2" xfId="35"/>
-    <cellStyle name="Column heading" xfId="36"/>
-    <cellStyle name="Comma 2" xfId="37"/>
-    <cellStyle name="Comma 2 2" xfId="38"/>
-    <cellStyle name="Comma 3" xfId="39"/>
-    <cellStyle name="Comma 4" xfId="40"/>
-    <cellStyle name="Comma 5" xfId="41"/>
-    <cellStyle name="Comma 6" xfId="42"/>
-    <cellStyle name="Comma 7" xfId="43"/>
-    <cellStyle name="Comma 8" xfId="44"/>
-    <cellStyle name="Corner heading" xfId="45"/>
-    <cellStyle name="Currency 2" xfId="46"/>
-    <cellStyle name="Currency 3" xfId="47"/>
-    <cellStyle name="Currency 3 2" xfId="48"/>
-    <cellStyle name="Data" xfId="49"/>
-    <cellStyle name="Data 2" xfId="50"/>
-    <cellStyle name="Data no deci" xfId="51"/>
-    <cellStyle name="Data Superscript" xfId="52"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="53"/>
-    <cellStyle name="Explanatory Text 2" xfId="54"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55"/>
-    <cellStyle name="Footnotes: top row" xfId="2"/>
-    <cellStyle name="Footnotes: top row 2" xfId="56"/>
-    <cellStyle name="Good 2" xfId="57"/>
-    <cellStyle name="Header: bottom row" xfId="5"/>
-    <cellStyle name="Header: bottom row 2" xfId="58"/>
-    <cellStyle name="Heading 1 2" xfId="59"/>
-    <cellStyle name="Heading 2 2" xfId="60"/>
-    <cellStyle name="Heading 3 2" xfId="61"/>
-    <cellStyle name="Heading 4 2" xfId="62"/>
-    <cellStyle name="Hed Side" xfId="63"/>
-    <cellStyle name="Hed Side 2" xfId="64"/>
-    <cellStyle name="Hed Side bold" xfId="65"/>
-    <cellStyle name="Hed Side Indent" xfId="66"/>
-    <cellStyle name="Hed Side Regular" xfId="67"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="68"/>
-    <cellStyle name="Hed Top" xfId="69"/>
-    <cellStyle name="Hed Top - SECTION" xfId="70"/>
-    <cellStyle name="Hed Top_3-new4" xfId="71"/>
-    <cellStyle name="Hyperlink 2" xfId="72"/>
-    <cellStyle name="Input 2" xfId="73"/>
-    <cellStyle name="Linked Cell 2" xfId="74"/>
-    <cellStyle name="Neutral 2" xfId="75"/>
+    <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Accent1 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Accent2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Accent3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Accent4 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Accent5 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Accent6 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Bad 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Body: normal cell 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Calculation 2" xfId="34" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Check Cell 2" xfId="35" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Column heading" xfId="36" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Comma 2" xfId="37" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Comma 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Comma 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Comma 4" xfId="40" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Comma 5" xfId="41" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Comma 6" xfId="42" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Comma 7" xfId="43" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Comma 8" xfId="44" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Corner heading" xfId="45" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Currency 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Currency 3" xfId="47" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Currency 3 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Data" xfId="49" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Data 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Data no deci" xfId="51" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Data Superscript" xfId="52" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="53" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Footnotes: top row 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Good 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Header: bottom row 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Heading 1 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Heading 2 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Heading 3 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Heading 4 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Hed Side" xfId="63" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Hed Side 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Hed Side bold" xfId="65" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Hed Side Indent" xfId="66" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="68" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Hed Top" xfId="69" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Hed Top - SECTION" xfId="70" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Hed Top_3-new4" xfId="71" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Input 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Neutral 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="76"/>
-    <cellStyle name="Normal 11" xfId="77"/>
-    <cellStyle name="Normal 12" xfId="153"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="78"/>
-    <cellStyle name="Normal 2 3" xfId="79"/>
-    <cellStyle name="Normal 3" xfId="80"/>
-    <cellStyle name="Normal 3 2" xfId="81"/>
-    <cellStyle name="Normal 3 2 2" xfId="82"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="83"/>
-    <cellStyle name="Normal 3 2 3" xfId="84"/>
-    <cellStyle name="Normal 3 3" xfId="85"/>
-    <cellStyle name="Normal 3 3 2" xfId="86"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="87"/>
-    <cellStyle name="Normal 3 3 3" xfId="88"/>
-    <cellStyle name="Normal 3 4" xfId="89"/>
-    <cellStyle name="Normal 3 4 2" xfId="90"/>
-    <cellStyle name="Normal 3 5" xfId="91"/>
-    <cellStyle name="Normal 3 6" xfId="92"/>
-    <cellStyle name="Normal 3 7" xfId="93"/>
-    <cellStyle name="Normal 4" xfId="94"/>
-    <cellStyle name="Normal 4 2" xfId="95"/>
-    <cellStyle name="Normal 4 2 2" xfId="96"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="97"/>
-    <cellStyle name="Normal 4 2 3" xfId="98"/>
-    <cellStyle name="Normal 4 3" xfId="99"/>
-    <cellStyle name="Normal 4 3 2" xfId="100"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="101"/>
-    <cellStyle name="Normal 4 3 3" xfId="102"/>
-    <cellStyle name="Normal 4 4" xfId="103"/>
-    <cellStyle name="Normal 4 4 2" xfId="104"/>
-    <cellStyle name="Normal 4 5" xfId="105"/>
-    <cellStyle name="Normal 4 6" xfId="106"/>
-    <cellStyle name="Normal 4 7" xfId="107"/>
-    <cellStyle name="Normal 5" xfId="108"/>
-    <cellStyle name="Normal 5 2" xfId="109"/>
-    <cellStyle name="Normal 5 3" xfId="110"/>
-    <cellStyle name="Normal 6" xfId="111"/>
-    <cellStyle name="Normal 6 2" xfId="112"/>
-    <cellStyle name="Normal 7" xfId="113"/>
-    <cellStyle name="Normal 7 2" xfId="114"/>
-    <cellStyle name="Normal 8" xfId="115"/>
-    <cellStyle name="Normal 9" xfId="116"/>
-    <cellStyle name="Note 2" xfId="117"/>
-    <cellStyle name="Note 2 2" xfId="118"/>
-    <cellStyle name="Output 2" xfId="119"/>
-    <cellStyle name="Parent row" xfId="3"/>
-    <cellStyle name="Parent row 2" xfId="120"/>
-    <cellStyle name="Percent 2" xfId="121"/>
-    <cellStyle name="Percent 2 2" xfId="122"/>
-    <cellStyle name="Percent 3" xfId="123"/>
-    <cellStyle name="Percent 3 2" xfId="124"/>
-    <cellStyle name="Percent 4" xfId="125"/>
-    <cellStyle name="Reference" xfId="126"/>
-    <cellStyle name="Row heading" xfId="127"/>
-    <cellStyle name="Source Hed" xfId="128"/>
-    <cellStyle name="Source Letter" xfId="129"/>
-    <cellStyle name="Source Superscript" xfId="130"/>
-    <cellStyle name="Source Superscript 2" xfId="131"/>
-    <cellStyle name="Source Text" xfId="132"/>
-    <cellStyle name="Source Text 2" xfId="133"/>
-    <cellStyle name="State" xfId="134"/>
-    <cellStyle name="Superscript" xfId="135"/>
-    <cellStyle name="Table Data" xfId="136"/>
-    <cellStyle name="Table Head Top" xfId="137"/>
-    <cellStyle name="Table Hed Side" xfId="138"/>
-    <cellStyle name="Table title" xfId="7"/>
-    <cellStyle name="Table title 2" xfId="139"/>
-    <cellStyle name="Title 2" xfId="140"/>
-    <cellStyle name="Title Text" xfId="141"/>
-    <cellStyle name="Title Text 1" xfId="142"/>
-    <cellStyle name="Title Text 2" xfId="143"/>
-    <cellStyle name="Title-1" xfId="144"/>
-    <cellStyle name="Title-2" xfId="145"/>
-    <cellStyle name="Title-3" xfId="146"/>
-    <cellStyle name="Total 2" xfId="147"/>
-    <cellStyle name="Warning Text 2" xfId="148"/>
-    <cellStyle name="Wrap" xfId="149"/>
-    <cellStyle name="Wrap Bold" xfId="150"/>
-    <cellStyle name="Wrap Title" xfId="151"/>
-    <cellStyle name="Wrap_NTS99-~11" xfId="152"/>
+    <cellStyle name="Normal 10" xfId="76" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Normal 11" xfId="77" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 12" xfId="153" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 3 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 3 2 3" xfId="84" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 3 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 3 3 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 3 3 3" xfId="88" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 3 4" xfId="89" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 3 4 2" xfId="90" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 3 5" xfId="91" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 3 6" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 3 7" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 4" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 4 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 4 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 4 2 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 4 3" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 4 3 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 4 3 3" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 4 4" xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 4 4 2" xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 4 5" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 4 6" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 4 7" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 5" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 5 2" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 5 3" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 6" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 6 2" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 7" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 7 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 8" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 9" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Note 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Note 2 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Output 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Parent row 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Percent 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Percent 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Percent 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Percent 3 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Percent 4" xfId="125" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Reference" xfId="126" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Row heading" xfId="127" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Source Hed" xfId="128" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Source Letter" xfId="129" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Source Superscript" xfId="130" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Source Superscript 2" xfId="131" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Source Text" xfId="132" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Source Text 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="State" xfId="134" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Superscript" xfId="135" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Table Data" xfId="136" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Table Head Top" xfId="137" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Table Hed Side" xfId="138" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Table title 2" xfId="139" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Title 2" xfId="140" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Title Text" xfId="141" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Title Text 1" xfId="142" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Title Text 2" xfId="143" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Title-1" xfId="144" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Title-2" xfId="145" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Title-3" xfId="146" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Total 2" xfId="147" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Warning Text 2" xfId="148" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Wrap" xfId="149" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Wrap Bold" xfId="150" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Wrap Title" xfId="151" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Wrap_NTS99-~11" xfId="152" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1439,6 +1440,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1474,6 +1492,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1649,14 +1684,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A15"/>
+    <sheetView tabSelected="1" zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
+      <selection activeCell="BH73" sqref="BH73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="2" max="2" width="107.33203125" customWidth="1"/>
@@ -1728,7 +1763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1738,12 +1773,12 @@
       <selection activeCell="C2" sqref="C2:AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -2812,7 +2847,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -2822,12 +2857,12 @@
       <selection activeCell="C2" sqref="C2:AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -3896,7 +3931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -3906,12 +3941,12 @@
       <selection activeCell="C2" sqref="C2:AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -4021,135 +4056,135 @@
       </c>
       <c r="B2" s="2">
         <f>SYFAFE!F31</f>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="C2" s="2">
         <f>B2</f>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:AH8" si="0">C2</f>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="J2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="L2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="N2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="O2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="P2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="Q2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="R2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="S2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="T2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="U2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="V2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="W2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="X2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="Y2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="Z2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="AA2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="AB2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="AC2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="AD2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="AE2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="AF2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="AG2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="AH2" s="2">
         <f t="shared" si="0"/>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -4158,135 +4193,135 @@
       </c>
       <c r="B3" s="2">
         <f>SYFAFE!F32</f>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:R8" si="1">B3</f>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="N3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="O3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="P3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="Q3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="R3" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="S3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="T3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="U3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="V3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="X3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="Y3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="Z3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AA3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AB3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AC3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AD3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AE3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AF3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AG3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AH3" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -4295,135 +4330,135 @@
       </c>
       <c r="B4" s="2">
         <f>SYFAFE!F33</f>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="P4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="Q4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="R4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="S4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="T4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="U4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="V4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="W4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="X4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="Y4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="Z4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AA4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AB4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AC4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AD4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AE4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AF4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AG4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AH4" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -4432,135 +4467,135 @@
       </c>
       <c r="B5" s="2">
         <f>SYFAFE!F34</f>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="1"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="P5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="Q5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="R5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="S5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="T5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="U5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="V5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="W5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="X5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="Y5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="Z5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AA5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AB5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AC5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AD5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AE5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AF5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AG5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="AH5" s="2">
         <f t="shared" si="0"/>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
     </row>
     <row r="6" spans="1:34">
@@ -4843,135 +4878,135 @@
       </c>
       <c r="B8" s="2">
         <f>SYFAFE!F37</f>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="R8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="S8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="T8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="U8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="V8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="W8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="X8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="Y8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="Z8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="AA8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="AB8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="AC8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="AD8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="AE8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="AF8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="AG8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="AH8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
     </row>
   </sheetData>
@@ -4980,7 +5015,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -4990,12 +5025,12 @@
       <selection activeCell="C2" sqref="C2:AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -5105,135 +5140,135 @@
       </c>
       <c r="B2" s="2">
         <f>SYFAFE!G22</f>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="C2" s="2">
         <f>B2</f>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:AH8" si="0">C2</f>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="J2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="L2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="N2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="O2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="P2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="Q2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="R2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="S2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="T2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="U2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="V2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="W2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="X2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="Y2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="Z2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="AA2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="AB2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="AC2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="AD2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="AE2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="AF2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="AG2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="AH2" s="2">
         <f t="shared" si="0"/>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -5242,135 +5277,135 @@
       </c>
       <c r="B3" s="2">
         <f>SYFAFE!G23</f>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:R8" si="1">B3</f>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="N3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="O3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="P3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="Q3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="R3" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="S3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="T3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="U3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="V3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="X3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="Y3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="Z3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AA3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AB3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AC3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AD3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AE3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AF3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AG3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AH3" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -5379,135 +5414,135 @@
       </c>
       <c r="B4" s="2">
         <f>SYFAFE!G24</f>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="P4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="Q4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="R4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="S4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="T4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="U4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="V4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="W4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="X4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="Y4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="Z4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AA4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AB4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AC4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AD4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AE4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AF4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AG4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AH4" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -5516,135 +5551,135 @@
       </c>
       <c r="B5" s="2">
         <f>SYFAFE!G25</f>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="1"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="P5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="Q5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="R5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="S5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="T5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="U5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="V5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="W5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="X5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="Y5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="Z5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AA5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AB5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AC5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AD5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AE5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AF5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AG5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="AH5" s="2">
         <f t="shared" si="0"/>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
     </row>
     <row r="6" spans="1:34">
@@ -5653,135 +5688,135 @@
       </c>
       <c r="B6" s="2">
         <f>SYFAFE!G26</f>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="1"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="O6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="P6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="Q6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="R6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="S6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="T6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="U6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="V6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="W6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="X6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="Y6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="Z6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="AA6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="AB6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="AC6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="AD6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="AE6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="AF6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="AG6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="AH6" s="2">
         <f t="shared" si="0"/>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
     </row>
     <row r="7" spans="1:34">
@@ -5790,135 +5825,135 @@
       </c>
       <c r="B7" s="2">
         <f>SYFAFE!G27</f>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="P7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="Q7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="R7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="S7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="T7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="U7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="V7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="W7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="X7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="Y7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="Z7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="AA7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="AB7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="AC7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="AD7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="AE7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="AF7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="AG7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="AH7" s="2">
         <f t="shared" si="0"/>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
     </row>
     <row r="8" spans="1:34">
@@ -5927,135 +5962,135 @@
       </c>
       <c r="B8" s="2">
         <f>SYFAFE!G28</f>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="R8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="S8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="T8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="U8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="V8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="W8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="X8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="Y8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="Z8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="AA8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="AB8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="AC8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="AD8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="AE8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="AF8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="AG8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
       <c r="AH8" s="2">
         <f t="shared" si="0"/>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
     </row>
   </sheetData>
@@ -6064,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -6074,12 +6109,12 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -6917,18 +6952,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="25" style="8" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="15.796875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="8" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="8" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" style="8" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="8" customWidth="1"/>
@@ -6937,7 +6972,7 @@
     <col min="9" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" ht="14.25">
+    <row r="1" spans="1:8" s="14" customFormat="1" ht="15">
       <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
@@ -6949,7 +6984,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8" ht="28.5">
+    <row r="2" spans="1:8" ht="32">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -6975,7 +7010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.25">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -7001,21 +7036,21 @@
         <v>8.3199999999999995E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.25">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="10">
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="C4" s="10">
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="D4" s="11">
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="E4" s="11">
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="F4" s="11">
         <v>0</v>
@@ -7024,10 +7059,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="11">
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.25">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -7053,21 +7088,21 @@
         <v>1.3979999999999997E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="10">
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="C6" s="10">
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="D6" s="10">
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="E6" s="11">
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -7076,10 +7111,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="11">
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.25">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -7105,33 +7140,33 @@
         <v>2.1378171339705042E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="10">
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
       <c r="C8" s="10">
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="D8" s="11">
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="E8" s="11">
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
       <c r="F8" s="11">
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
       <c r="G8" s="11">
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
       <c r="H8" s="11">
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="14" t="s">
         <v>24</v>
       </c>
@@ -7157,7 +7192,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="14" t="s">
         <v>10</v>
       </c>
@@ -7183,7 +7218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="14" t="s">
         <v>8</v>
       </c>
@@ -7209,7 +7244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="14" t="s">
         <v>7</v>
       </c>
@@ -7235,7 +7270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.25">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="14" t="s">
         <v>11</v>
       </c>
@@ -7261,21 +7296,21 @@
         <v>5.4986866418063425E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="14">
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="C16" s="14">
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="D16" s="14">
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="E16" s="14">
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="F16" s="14">
         <v>0</v>
@@ -7284,10 +7319,10 @@
         <v>0</v>
       </c>
       <c r="H16" s="14">
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.25">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="14" t="s">
         <v>13</v>
       </c>
@@ -7325,7 +7360,7 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" ht="28.5">
+    <row r="21" spans="1:8" ht="32">
       <c r="A21" s="7" t="s">
         <v>23</v>
       </c>
@@ -7348,7 +7383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.25">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="9" t="s">
         <v>2</v>
       </c>
@@ -7358,7 +7393,7 @@
       </c>
       <c r="C22" s="10">
         <f>B4</f>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="D22" s="10">
         <f>B5</f>
@@ -7366,7 +7401,7 @@
       </c>
       <c r="E22" s="10">
         <f>B6</f>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="F22" s="10">
         <f>B7</f>
@@ -7374,10 +7409,10 @@
       </c>
       <c r="G22" s="10">
         <f>B8</f>
-        <v>6.7858445582245526E-3</v>
+        <v>2.8218046646878922E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.25">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="9" t="s">
         <v>3</v>
       </c>
@@ -7387,7 +7422,7 @@
       </c>
       <c r="C23" s="10">
         <f>C4</f>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="D23" s="10">
         <f>C5</f>
@@ -7395,7 +7430,7 @@
       </c>
       <c r="E23" s="10">
         <f>C6</f>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="F23" s="10">
         <f>C7</f>
@@ -7403,10 +7438,10 @@
       </c>
       <c r="G23" s="10">
         <f>C8</f>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.25">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="9" t="s">
         <v>4</v>
       </c>
@@ -7416,7 +7451,7 @@
       </c>
       <c r="C24" s="11">
         <f>D4</f>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="D24" s="10">
         <f>D5</f>
@@ -7424,7 +7459,7 @@
       </c>
       <c r="E24" s="10">
         <f>D6</f>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="F24" s="10">
         <f>D7</f>
@@ -7432,10 +7467,10 @@
       </c>
       <c r="G24" s="11">
         <f>D8</f>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.25">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="9" t="s">
         <v>5</v>
       </c>
@@ -7445,7 +7480,7 @@
       </c>
       <c r="C25" s="11">
         <f>E4</f>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="D25" s="11">
         <f>E5</f>
@@ -7453,7 +7488,7 @@
       </c>
       <c r="E25" s="11">
         <f>E6</f>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="F25" s="11">
         <f>E7</f>
@@ -7461,10 +7496,10 @@
       </c>
       <c r="G25" s="11">
         <f>E8</f>
-        <v>2.1310916794424219E-3</v>
+        <v>8.8618658891024735E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.25">
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="9" t="s">
         <v>6</v>
       </c>
@@ -7490,10 +7525,10 @@
       </c>
       <c r="G26" s="11">
         <f>F8</f>
-        <v>4.6912057627725937E-3</v>
+        <v>1.950776530587952E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.25">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="9" t="s">
         <v>20</v>
       </c>
@@ -7519,10 +7554,10 @@
       </c>
       <c r="G27" s="11">
         <f>G8</f>
-        <v>1.6515960515678771E-3</v>
+        <v>6.8679460640544171E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.25">
+    <row r="28" spans="1:8" ht="15">
       <c r="A28" s="9" t="s">
         <v>21</v>
       </c>
@@ -7532,7 +7567,7 @@
       </c>
       <c r="C28" s="11">
         <f>H4</f>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="D28" s="11">
         <f>H5</f>
@@ -7540,7 +7575,7 @@
       </c>
       <c r="E28" s="11">
         <f>H6</f>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="F28" s="11">
         <f>H7</f>
@@ -7548,10 +7583,10 @@
       </c>
       <c r="G28" s="11">
         <f>H8</f>
-        <v>6.3932750383272645E-3</v>
+        <v>2.6585597667307418E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="28.5">
+    <row r="30" spans="1:8" ht="32">
       <c r="A30" s="7" t="s">
         <v>24</v>
       </c>
@@ -7574,7 +7609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.25">
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="14" t="s">
         <v>2</v>
       </c>
@@ -7596,14 +7631,14 @@
       </c>
       <c r="F31" s="14">
         <f>B16</f>
-        <v>1.580720948786267E-2</v>
+        <v>0.10723822440351093</v>
       </c>
       <c r="G31" s="14">
         <f>B17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="14.25">
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="14" t="s">
         <v>3</v>
       </c>
@@ -7625,14 +7660,14 @@
       </c>
       <c r="F32" s="14">
         <f>C16</f>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="G32" s="14">
         <f>C17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14.25">
+    <row r="33" spans="1:7" ht="15">
       <c r="A33" s="14" t="s">
         <v>4</v>
       </c>
@@ -7654,14 +7689,14 @@
       </c>
       <c r="F33" s="14">
         <f>D16</f>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="G33" s="14">
         <f>D17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14.25">
+    <row r="34" spans="1:7" ht="15">
       <c r="A34" s="14" t="s">
         <v>5</v>
       </c>
@@ -7683,14 +7718,14 @@
       </c>
       <c r="F34" s="14">
         <f>E16</f>
-        <v>4.9190397487553798E-3</v>
+        <v>3.337142389565087E-2</v>
       </c>
       <c r="G34" s="14">
         <f>E17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="14.25">
+    <row r="35" spans="1:7" ht="15">
       <c r="A35" s="14" t="s">
         <v>6</v>
       </c>
@@ -7719,7 +7754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="14.25">
+    <row r="36" spans="1:7" ht="15">
       <c r="A36" s="14" t="s">
         <v>20</v>
       </c>
@@ -7748,7 +7783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14.25">
+    <row r="37" spans="1:7" ht="15">
       <c r="A37" s="14" t="s">
         <v>21</v>
       </c>
@@ -7770,7 +7805,7 @@
       </c>
       <c r="F37" s="14">
         <f>H16</f>
-        <v>1.4757119246266137E-2</v>
+        <v>0.1001142716869526</v>
       </c>
       <c r="G37" s="14">
         <f>H17</f>
@@ -7784,7 +7819,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -7794,12 +7829,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -8868,7 +8903,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -8878,12 +8913,12 @@
       <selection activeCell="B2" sqref="B2:AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -9721,7 +9756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -9731,12 +9766,12 @@
       <selection activeCell="C2" sqref="C2:AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -9846,135 +9881,135 @@
       </c>
       <c r="B2" s="2">
         <f>SYFAFE!C22</f>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="C2" s="2">
         <f>B2</f>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:AH8" si="0">C2</f>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="J2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="L2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="N2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="O2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="P2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="Q2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="R2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="S2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="T2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="U2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="V2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="W2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="X2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="Y2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="Z2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="AA2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="AB2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="AC2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="AD2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="AE2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="AF2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="AG2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
       <c r="AH2" s="2">
         <f t="shared" si="0"/>
-        <v>1.362816616770287E-3</v>
+        <v>7.9588997630576728E-4</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -9983,135 +10018,135 @@
       </c>
       <c r="B3" s="2">
         <f>SYFAFE!C23</f>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:R8" si="1">B3</f>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="N3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="O3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="P3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="Q3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="R3" s="2">
         <f t="shared" si="1"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="S3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="T3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="U3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="V3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="X3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="Y3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="Z3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="AA3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="AB3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="AC3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="AD3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="AE3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="AF3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="AG3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
       <c r="AH3" s="2">
         <f t="shared" si="0"/>
-        <v>1.79343314551659E-3</v>
+        <v>1.792469118457498E-3</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -10120,135 +10155,135 @@
       </c>
       <c r="B4" s="2">
         <f>SYFAFE!C24</f>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="1"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="P4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="Q4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="R4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="S4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="T4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="U4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="V4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="W4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="X4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="Y4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="Z4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="AA4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="AB4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="AC4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="AD4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="AE4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="AF4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="AG4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
       <c r="AH4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5590676482152321E-4</v>
+        <v>1.559080400922843E-4</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -10257,135 +10292,135 @@
       </c>
       <c r="B5" s="2">
         <f>SYFAFE!C25</f>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="1"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="P5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="Q5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="R5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="S5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="T5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="U5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="V5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="W5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="X5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="Y5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="Z5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="AA5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="AB5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="AC5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="AD5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="AE5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="AF5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="AG5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
       <c r="AH5" s="2">
         <f t="shared" si="0"/>
-        <v>8.0444857169030375E-4</v>
+        <v>8.0410948504312872E-4</v>
       </c>
     </row>
     <row r="6" spans="1:34">
@@ -10668,135 +10703,135 @@
       </c>
       <c r="B8" s="2">
         <f>SYFAFE!C28</f>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="R8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="S8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="T8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="U8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="V8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="W8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="X8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="Y8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="Z8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="AA8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="AB8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="AC8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="AD8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="AE8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="AF8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="AG8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
       <c r="AH8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4133457150709108E-3</v>
+        <v>2.4123284551293856E-3</v>
       </c>
     </row>
   </sheetData>
@@ -10805,7 +10840,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -10815,12 +10850,12 @@
       <selection activeCell="C2" sqref="C2:AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -11889,7 +11924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -11899,12 +11934,12 @@
       <selection activeCell="C2" sqref="C2:AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -12973,7 +13008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -12983,12 +13018,12 @@
       <selection activeCell="B2" sqref="B2:AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -13826,7 +13861,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -13836,12 +13871,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -13951,135 +13986,135 @@
       </c>
       <c r="B2" s="2">
         <f>SYFAFE!E22</f>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="C2" s="2">
         <f>B2</f>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" ref="D2:AH8" si="0">C2</f>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="J2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="L2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="N2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="O2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="P2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="Q2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="R2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="S2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="T2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="U2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="V2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="W2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="X2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="Y2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="Z2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="AA2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="AB2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="AC2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="AD2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="AE2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="AF2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="AG2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
       <c r="AH2" s="2">
         <f t="shared" si="0"/>
-        <v>1.397782879998018E-3</v>
+        <v>1.360594417697611E-3</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -14088,135 +14123,135 @@
       </c>
       <c r="B3" s="2">
         <f>SYFAFE!E23</f>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:R8" si="1">B3</f>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="N3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="O3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="P3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="Q3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="R3" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="S3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="T3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="U3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="V3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="X3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="Y3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="Z3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AA3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AB3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AC3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AD3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AE3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AF3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AG3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AH3" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -14225,135 +14260,135 @@
       </c>
       <c r="B4" s="2">
         <f>SYFAFE!E24</f>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="P4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="Q4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="R4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="S4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="T4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="U4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="V4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="W4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="X4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="Y4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="Z4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AA4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AB4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AC4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AD4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AE4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AF4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AG4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AH4" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -14362,135 +14397,135 @@
       </c>
       <c r="B5" s="2">
         <f>SYFAFE!E25</f>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="1"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="P5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="Q5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="R5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="S5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="T5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="U5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="V5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="W5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="X5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="Y5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="Z5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AA5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AB5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AC5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AD5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AE5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AF5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AG5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
       <c r="AH5" s="2">
         <f t="shared" si="0"/>
-        <v>4.8101686276135923E-4</v>
+        <v>4.6821925469029281E-4</v>
       </c>
     </row>
     <row r="6" spans="1:34">
@@ -14773,135 +14808,135 @@
       </c>
       <c r="B8" s="2">
         <f>SYFAFE!E28</f>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="R8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="S8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="T8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="U8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="V8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="W8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="X8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="Y8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="Z8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="AA8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="AB8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="AC8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="AD8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="AE8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="AF8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="AG8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
       <c r="AH8" s="2">
         <f t="shared" si="0"/>
-        <v>1.4430505882840775E-3</v>
+        <v>1.4046577640708783E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>